<commit_message>
All files for assessment added
Boxplot-WebG.png and cso_image.png added just in case they were missing

Thre python file with calculations present 
MSC DA CA1 - Exploratory Data Analysis.ipynb updated graphs with titles and better data preparation
MSC DA CA1 - Statistics .ipynb updated graphs with titles and better data preparation
MSC DA CA1 - Machine Learning.ipynb this file may be reuploaded if some progress is made

MSC DA CA1.docx all questions attempted 
PEA25_estimated_population.xlsx chosen dataset
</commit_message>
<xml_diff>
--- a/PEA25_estimated_population.xlsx
+++ b/PEA25_estimated_population.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stphn\Documents\CCT\Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF87B247-B5BE-458A-8C83-5DD5FE7D344C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2787D9-0E47-482E-A42A-FF04FA1D9436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Stephen Kelly" refreshedDate="45246.959425347224" createdVersion="5" refreshedVersion="8" minRefreshableVersion="3" recordCount="324" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Stephen Kelly" refreshedDate="45247.484961689814" createdVersion="5" refreshedVersion="8" minRefreshableVersion="3" recordCount="324" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F325" sheet="Unpivoted"/>
   </cacheSource>
@@ -4837,8 +4837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="F308" sqref="F308"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>